<commit_message>
Extent + Screenshot fully functional - Added CalendarPage, CallsPage, CampaignsPage, CasePage, CompaniesPage, ContactsPage, DealsPage, DocumentsPage, EmailPage, FormsPage
</commit_message>
<xml_diff>
--- a/src/main/java/testData/TestData1.xlsx
+++ b/src/main/java/testData/TestData1.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sami\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sami\IdeaProjects\CogmentoCRM\src\main\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{645EA089-06BD-491B-B93B-ED0B4A30E94D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6678F54C-0B88-42F7-9C0A-ABDAD41ABF18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{146A2D8D-17AB-41AF-8F70-7C7CC415B18A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{146A2D8D-17AB-41AF-8F70-7C7CC415B18A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="LoginPageLeftSidebarLinks" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Username</t>
   </si>
@@ -63,13 +64,46 @@
     <t>kkumar@gmail.com</t>
   </si>
   <si>
-    <t>ameikh645@gmail.com</t>
-  </si>
-  <si>
-    <t>Tripleh1!</t>
-  </si>
-  <si>
     <t>123Pass</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com/home</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com/calendar</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com/contacts</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com/companies</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com/deals</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com/tasks</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com/cases</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com/calls</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com/documents</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com/email</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com/campaigns</t>
+  </si>
+  <si>
+    <t>https://ui.cogmento.com/forms</t>
   </si>
 </sst>
 </file>
@@ -441,9 +475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B23AC55-A9C9-42DD-BB1C-7870012BABBD}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -487,16 +519,11 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
+      <c r="A6" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -504,8 +531,87 @@
     <hyperlink ref="A3" r:id="rId2" xr:uid="{E961671D-F952-44E5-89CE-A1A4CDC60C01}"/>
     <hyperlink ref="A4" r:id="rId3" xr:uid="{3FC20CE7-4B32-4A42-8EDE-669A8D4DBB88}"/>
     <hyperlink ref="A5" r:id="rId4" xr:uid="{0514285E-0087-4021-A420-A3FBB894EF61}"/>
-    <hyperlink ref="A6" r:id="rId5" xr:uid="{298D008F-A879-4D30-B054-AB59B90A55A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0591BAEC-15AB-44C4-843A-E35584234A03}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Sync + ton of additional project structure + classes
</commit_message>
<xml_diff>
--- a/src/main/java/testData/TestData1.xlsx
+++ b/src/main/java/testData/TestData1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sami\IdeaProjects\CogmentoCRM\src\main\java\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6678F54C-0B88-42F7-9C0A-ABDAD41ABF18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8F94EC-41C8-42B2-A07B-FC318A3490D4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="1" xr2:uid="{146A2D8D-17AB-41AF-8F70-7C7CC415B18A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{146A2D8D-17AB-41AF-8F70-7C7CC415B18A}"/>
   </bookViews>
   <sheets>
     <sheet name="InvalidLogin" sheetId="1" r:id="rId1"/>
     <sheet name="LoginPageLeftSidebarLinks" sheetId="2" r:id="rId2"/>
+    <sheet name="CreateNewEventFormTitles" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Username</t>
   </si>
@@ -104,6 +105,66 @@
   </si>
   <si>
     <t>https://ui.cogmento.com/forms</t>
+  </si>
+  <si>
+    <t>Form Titles</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Calendar</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>All Day</t>
+  </si>
+  <si>
+    <t>Deal</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Case</t>
+  </si>
+  <si>
+    <t>Alert</t>
+  </si>
+  <si>
+    <t>Reminder Time</t>
+  </si>
+  <si>
+    <t>Assigned To</t>
+  </si>
+  <si>
+    <t>Participants</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Recurrence</t>
+  </si>
+  <si>
+    <t>Identifier</t>
   </si>
 </sst>
 </file>
@@ -540,7 +601,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0591BAEC-15AB-44C4-843A-E35584234A03}">
   <dimension ref="A1:A13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -614,4 +675,122 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F469D72F-38D1-4953-96EA-477A110B8F16}">
+  <dimension ref="A1:A20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>